<commit_message>
update rka dari web
</commit_message>
<xml_diff>
--- a/data/rka.xlsx
+++ b/data/rka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KAI\Data\ZFM01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AC50C813-64F4-4186-B977-B3A51CD57006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{46B1F74C-F976-48B7-9162-2A67BD403BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975"/>
   </bookViews>
@@ -1248,8 +1248,8 @@
   <dimension ref="A1:H543"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A421" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G436" sqref="G436"/>
+      <pane ySplit="1" topLeftCell="A516" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:H543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14705,5 +14705,6 @@
   </sheetData>
   <autoFilter ref="A1:H543"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>